<commit_message>
Updated the test plan and documentation README.md
</commit_message>
<xml_diff>
--- a/doc/TestPlan/TestPlanSheet.xlsx
+++ b/doc/TestPlan/TestPlanSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IGMProfile\Desktop\Infiltrator_D\doc\TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profiles\sj6045\IGME-601-2181-Team-C\doc\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Instructions</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Given that guards are supposed to protect the information player wants to still they should perform random patrols to keep an eye on enviornment.</t>
   </si>
   <si>
-    <t>Given that guards can be distracted by the noise they should be able to move to the origin of sound flawlessly (Create a framework to add these listeners for guards).</t>
-  </si>
-  <si>
     <t>As a Player I want to press a button while near a wall socket so that I can plug in and gain energy over time.</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>MD 10/29 Didn't get to this implementation yet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that guards can detect player (either by sight or sound), when detected they move towards the player/suspicious spot flawlessly. </t>
+  </si>
+  <si>
+    <t>SJ 10/29 (Implemented with the sight detection.Sound detection yet to be implemented)</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -372,6 +375,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -392,6 +409,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -412,6 +443,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -432,6 +477,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -452,6 +511,104 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -468,478 +625,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1320,9 +1005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E15" sqref="E15"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1356,10 +1041,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1368,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1382,10 +1067,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1396,10 +1081,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1408,10 +1093,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1422,10 +1107,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1434,10 +1119,10 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1448,10 +1133,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1460,10 +1145,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1474,112 +1159,112 @@
         <v>23</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="C16" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3312,130 +2997,130 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3 C12 C20:C595 C6 C8 C14:C15 C10">
-    <cfRule type="cellIs" dxfId="13" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="81" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="82" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D10 D12 D14:D15 D20:D595">
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="75" stopIfTrue="1">
       <formula>AND(ISBLANK(D8),C8="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="76" stopIfTrue="1">
       <formula>AND(ISBLANK(D8),C8="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D3 D6">
-    <cfRule type="expression" dxfId="75" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="71" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="72" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="67" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="63" stopIfTrue="1">
       <formula>AND(ISBLANK(D4),C4="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="64" stopIfTrue="1">
       <formula>AND(ISBLANK(D4),C4="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="59" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="55" stopIfTrue="1">
       <formula>AND(ISBLANK(D5),C5="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="56" stopIfTrue="1">
       <formula>AND(ISBLANK(D5),C5="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="51" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="47" stopIfTrue="1">
       <formula>AND(ISBLANK(D7),C7="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="48" stopIfTrue="1">
       <formula>AND(ISBLANK(D7),C7="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="47" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="43" stopIfTrue="1">
       <formula>AND(ISBLANK(D11),C11="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="44" stopIfTrue="1">
       <formula>AND(ISBLANK(D11),C11="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="43" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="39" stopIfTrue="1">
       <formula>AND(ISBLANK(D13),C13="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="40" stopIfTrue="1">
       <formula>AND(ISBLANK(D13),C13="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="39" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="35" stopIfTrue="1">
       <formula>AND(ISBLANK(D17),C17="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="36" stopIfTrue="1">
       <formula>AND(ISBLANK(D17),C17="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
       <formula>AND(ISBLANK(D16),C16="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
       <formula>AND(ISBLANK(D16),C16="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="31" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="27" stopIfTrue="1">
       <formula>AND(ISBLANK(D19),C19="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="28" stopIfTrue="1">
       <formula>AND(ISBLANK(D19),C19="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="27" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
       <formula>AND(ISBLANK(D18),C18="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>AND(ISBLANK(D18),C18="Fail")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated the test case result for energy drain user story
</commit_message>
<xml_diff>
--- a/doc/TestPlan/TestPlanSheet.xlsx
+++ b/doc/TestPlan/TestPlanSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Instructions</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Given In a level when the game is unpaused then energy will go down.</t>
   </si>
   <si>
-    <t>Given In a level when I run out of energy then I will die.</t>
-  </si>
-  <si>
     <t xml:space="preserve">As a Player I want to see a beautiful 3D model of my drone when I am doing a mission so that I can have a more realistic flying experience. </t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>SJ 10/29 (Implemented with the sight detection.Sound detection yet to be implemented)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ 10/30 </t>
   </si>
 </sst>
 </file>
@@ -1003,11 +1003,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D595"/>
+  <dimension ref="A1:D594"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1041,10 +1041,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1067,10 +1067,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,10 +1081,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1093,10 +1093,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1107,10 +1107,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1119,10 +1119,10 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1133,10 +1133,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1145,10 +1145,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1159,22 +1159,22 @@
         <v>23</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1185,10 +1185,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1197,10 +1197,10 @@
         <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1209,13 +1209,13 @@
         <v>27</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
@@ -1223,49 +1223,40 @@
         <v>29</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="11" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>37</v>
-      </c>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" s="8"/>
@@ -2992,11 +2983,8 @@
     <row r="594" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C594" s="8"/>
     </row>
-    <row r="595" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C595" s="8"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C3 C12 C20:C595 C6 C8 C14:C15 C10">
+  <conditionalFormatting sqref="C2:C3 C12 C19:C594 C6 C8 C14:C15 C10">
     <cfRule type="cellIs" dxfId="43" priority="81" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3004,7 +2992,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D10 D12 D14:D15 D20:D595">
+  <conditionalFormatting sqref="D8:D10 D12 D14:D15 D19:D594">
     <cfRule type="expression" dxfId="41" priority="75" stopIfTrue="1">
       <formula>AND(ISBLANK(D8),C8="Pass")</formula>
     </cfRule>
@@ -3060,22 +3048,6 @@
       <formula>AND(ISBLANK(D13),C13="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="25" priority="35" stopIfTrue="1">
-      <formula>AND(ISBLANK(D17),C17="Pass")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="36" stopIfTrue="1">
-      <formula>AND(ISBLANK(D17),C17="Fail")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
       <formula>"Pass"</formula>
@@ -3092,7 +3064,7 @@
       <formula>AND(ISBLANK(D16),C16="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+  <conditionalFormatting sqref="C18">
     <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3100,15 +3072,15 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
+  <conditionalFormatting sqref="D18">
     <cfRule type="expression" dxfId="17" priority="27" stopIfTrue="1">
-      <formula>AND(ISBLANK(D19),C19="Pass")</formula>
+      <formula>AND(ISBLANK(D18),C18="Pass")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="28" stopIfTrue="1">
-      <formula>AND(ISBLANK(D19),C19="Fail")</formula>
+      <formula>AND(ISBLANK(D18),C18="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3116,12 +3088,12 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
+  <conditionalFormatting sqref="D17">
     <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
-      <formula>AND(ISBLANK(D18),C18="Pass")</formula>
+      <formula>AND(ISBLANK(D17),C17="Pass")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
-      <formula>AND(ISBLANK(D18),C18="Fail")</formula>
+      <formula>AND(ISBLANK(D17),C17="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
@@ -3173,7 +3145,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C595">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C594">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>